<commit_message>
minor changes to pytreesros numbers
</commit_message>
<xml_diff>
--- a/raw_model_data/py_trees_ros/py_trees_ros_codes_analysis.xlsx
+++ b/raw_model_data/py_trees_ros/py_trees_ros_codes_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Chalmers PhD\behaviortrees\raw_model_data\py_trees_ros\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Razan\Bitbucket\Behavior-Trees-in-Action\raw_model_data\py_trees_ros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CDA4F8-483C-4D2E-A096-6EB20E6C8676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6987E92A-DA2C-4DA5-A2D8-22EEB85F8465}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="python_codes_analysis" sheetId="1" r:id="rId1"/>
@@ -488,7 +488,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -670,12 +670,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -852,14 +846,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="35" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="34" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1222,133 +1216,133 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="69.42578125" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="30.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="30.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="32" customWidth="1"/>
-    <col min="12" max="12" width="22.33203125" customWidth="1"/>
-    <col min="13" max="13" width="21.109375" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="22.28515625" customWidth="1"/>
+    <col min="13" max="13" width="21.140625" hidden="1" customWidth="1"/>
     <col min="14" max="18" width="0" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="16.33203125" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="9.109375" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="16.28515625" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="0" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.6640625" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.7109375" hidden="1" customWidth="1"/>
     <col min="24" max="29" width="0" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="11.33203125" customWidth="1"/>
+    <col min="30" max="30" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AA1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AB1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AC1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AD1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AE1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AF1" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B2" t="s">
@@ -1361,7 +1355,7 @@
         <v>83</v>
       </c>
       <c r="E2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -1379,10 +1373,11 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>6</v>
+        <f t="shared" ref="K2:K21" si="0">SUM(E2:J2)</f>
+        <v>4</v>
       </c>
       <c r="L2">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="M2" s="1">
         <v>0.67</v>
@@ -1413,7 +1408,7 @@
       </c>
       <c r="V2">
         <f>SUM(K2:L2)</f>
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="W2" s="1">
         <v>0.22</v>
@@ -1440,15 +1435,16 @@
         <v>4</v>
       </c>
       <c r="AE2">
-        <v>18</v>
+        <f>SUM(K2:L2)</f>
+        <v>12</v>
       </c>
       <c r="AF2">
         <f>AVERAGE( 4,3,2,3,3,2)</f>
         <v>2.8333333333333335</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B3" t="s">
@@ -1479,6 +1475,7 @@
         <v>0</v>
       </c>
       <c r="K3">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="L3">
@@ -1512,7 +1509,7 @@
         <v>13</v>
       </c>
       <c r="V3">
-        <f t="shared" ref="V3:V21" si="0">SUM(K3:L3)</f>
+        <f t="shared" ref="V3:V21" si="1">SUM(K3:L3)</f>
         <v>15</v>
       </c>
       <c r="W3" s="1">
@@ -1540,6 +1537,7 @@
         <v>3</v>
       </c>
       <c r="AE3">
+        <f>SUM(K3:L3)</f>
         <v>15</v>
       </c>
       <c r="AF3">
@@ -1547,8 +1545,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>28</v>
       </c>
       <c r="B4" t="s">
@@ -1579,6 +1577,7 @@
         <v>0</v>
       </c>
       <c r="K4">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="L4">
@@ -1612,7 +1611,7 @@
         <v>6</v>
       </c>
       <c r="V4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="W4" s="1">
@@ -1640,6 +1639,7 @@
         <v>3</v>
       </c>
       <c r="AE4">
+        <f>SUM(K4:L4)</f>
         <v>8</v>
       </c>
       <c r="AF4">
@@ -1647,8 +1647,8 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>30</v>
       </c>
       <c r="B5" t="s">
@@ -1679,6 +1679,7 @@
         <v>0</v>
       </c>
       <c r="K5">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="L5">
@@ -1712,7 +1713,7 @@
         <v>8</v>
       </c>
       <c r="V5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="W5" s="1">
@@ -1740,6 +1741,7 @@
         <v>3</v>
       </c>
       <c r="AE5">
+        <f>SUM(K5:L5)</f>
         <v>12</v>
       </c>
       <c r="AF5">
@@ -1747,8 +1749,8 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>32</v>
       </c>
       <c r="B6" t="s">
@@ -1761,7 +1763,7 @@
         <v>83</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F6">
         <v>7</v>
@@ -1779,10 +1781,11 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <v>19</v>
+        <f>SUM(E6:J6)</f>
+        <v>20</v>
       </c>
       <c r="L6">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="M6" s="1">
         <v>0.16</v>
@@ -1812,8 +1815,8 @@
         <v>4</v>
       </c>
       <c r="V6">
-        <f t="shared" si="0"/>
-        <v>49</v>
+        <f t="shared" si="1"/>
+        <v>53</v>
       </c>
       <c r="W6" s="1">
         <v>0.06</v>
@@ -1840,15 +1843,16 @@
         <v>9</v>
       </c>
       <c r="AE6">
-        <v>49</v>
+        <f t="shared" ref="AE6:AE21" si="2">SUM(K6:L6)</f>
+        <v>53</v>
       </c>
       <c r="AF6">
         <f>AVERAGE(2,3,3,3,2,2,2,3,4,1,5,2,2,2,1,5,2,2,2)</f>
         <v>2.5263157894736841</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>35</v>
       </c>
       <c r="B7" t="s">
@@ -1879,6 +1883,7 @@
         <v>1</v>
       </c>
       <c r="K7">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="L7">
@@ -1912,7 +1917,7 @@
         <v>2</v>
       </c>
       <c r="V7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="W7" s="1">
@@ -1940,6 +1945,7 @@
         <v>5</v>
       </c>
       <c r="AE7">
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="AF7">
@@ -1947,8 +1953,8 @@
         <v>2.4285714285714284</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>38</v>
       </c>
       <c r="B8" t="s">
@@ -1979,10 +1985,11 @@
         <v>0</v>
       </c>
       <c r="K8">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="L8">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M8" s="1">
         <v>0.71</v>
@@ -2012,8 +2019,8 @@
         <v>2</v>
       </c>
       <c r="V8">
-        <f t="shared" si="0"/>
-        <v>19</v>
+        <f t="shared" si="1"/>
+        <v>18</v>
       </c>
       <c r="W8" s="1">
         <v>0.26</v>
@@ -2040,15 +2047,16 @@
         <v>5</v>
       </c>
       <c r="AE8">
-        <v>19</v>
+        <f t="shared" si="2"/>
+        <v>18</v>
       </c>
       <c r="AF8">
         <f>AVERAGE(2,3,4,2,3,2,2)</f>
         <v>2.5714285714285716</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>40</v>
       </c>
       <c r="B9" t="s">
@@ -2079,6 +2087,7 @@
         <v>0</v>
       </c>
       <c r="K9">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="L9">
@@ -2112,7 +2121,7 @@
         <v>3</v>
       </c>
       <c r="V9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="W9" s="1">
@@ -2140,6 +2149,7 @@
         <v>5</v>
       </c>
       <c r="AE9">
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="AF9">
@@ -2147,8 +2157,8 @@
         <v>2.875</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>42</v>
       </c>
       <c r="B10" t="s">
@@ -2179,6 +2189,7 @@
         <v>0</v>
       </c>
       <c r="K10">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="L10">
@@ -2212,7 +2223,7 @@
         <v>2</v>
       </c>
       <c r="V10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="W10" s="1">
@@ -2240,6 +2251,7 @@
         <v>5</v>
       </c>
       <c r="AE10">
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="AF10">
@@ -2247,8 +2259,8 @@
         <v>2.7142857142857144</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>44</v>
       </c>
       <c r="B11" t="s">
@@ -2279,10 +2291,11 @@
         <v>2</v>
       </c>
       <c r="K11">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="L11">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M11" s="1">
         <v>0.22</v>
@@ -2312,8 +2325,8 @@
         <v>5</v>
       </c>
       <c r="V11">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>21</v>
       </c>
       <c r="W11" s="1">
         <v>0.1</v>
@@ -2340,15 +2353,16 @@
         <v>6</v>
       </c>
       <c r="AE11">
-        <v>20</v>
+        <f t="shared" si="2"/>
+        <v>21</v>
       </c>
       <c r="AF11">
         <f>AVERAGE(2,3,3,2,3,2,2,2)</f>
         <v>2.375</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>46</v>
       </c>
       <c r="B12" t="s">
@@ -2379,6 +2393,7 @@
         <v>0</v>
       </c>
       <c r="K12">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="L12">
@@ -2412,7 +2427,7 @@
         <v>1</v>
       </c>
       <c r="V12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="W12" s="1">
@@ -2440,6 +2455,7 @@
         <v>5</v>
       </c>
       <c r="AE12">
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="AF12">
@@ -2447,8 +2463,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>48</v>
       </c>
       <c r="B13" t="s">
@@ -2479,6 +2495,7 @@
         <v>0</v>
       </c>
       <c r="K13">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="L13">
@@ -2512,7 +2529,7 @@
         <v>2</v>
       </c>
       <c r="V13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="W13" s="1">
@@ -2540,6 +2557,7 @@
         <v>4</v>
       </c>
       <c r="AE13">
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="AF13">
@@ -2547,8 +2565,8 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>50</v>
       </c>
       <c r="B14" t="s">
@@ -2579,6 +2597,7 @@
         <v>0</v>
       </c>
       <c r="K14">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="L14">
@@ -2612,7 +2631,7 @@
         <v>1</v>
       </c>
       <c r="V14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="W14" s="1">
@@ -2640,6 +2659,7 @@
         <v>4</v>
       </c>
       <c r="AE14">
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="AF14">
@@ -2647,8 +2667,8 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>52</v>
       </c>
       <c r="B15" t="s">
@@ -2679,6 +2699,7 @@
         <v>1</v>
       </c>
       <c r="K15">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="L15">
@@ -2712,7 +2733,7 @@
         <v>5</v>
       </c>
       <c r="V15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="W15" s="1">
@@ -2737,9 +2758,10 @@
         <v>0.63</v>
       </c>
       <c r="AD15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AE15">
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="AF15">
@@ -2747,8 +2769,8 @@
         <v>2.3333333333333335</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>55</v>
       </c>
       <c r="B16" t="s">
@@ -2761,13 +2783,13 @@
         <v>83</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -2779,7 +2801,8 @@
         <v>2</v>
       </c>
       <c r="K16">
-        <v>9</v>
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="L16">
         <v>20</v>
@@ -2812,8 +2835,8 @@
         <v>7</v>
       </c>
       <c r="V16">
-        <f t="shared" si="0"/>
-        <v>29</v>
+        <f t="shared" si="1"/>
+        <v>31</v>
       </c>
       <c r="W16" s="1">
         <v>0.14000000000000001</v>
@@ -2840,15 +2863,16 @@
         <v>6</v>
       </c>
       <c r="AE16">
-        <v>29</v>
+        <f t="shared" si="2"/>
+        <v>31</v>
       </c>
       <c r="AF16">
         <f>AVERAGE(2,6,5,2,2,2,2,2,5)</f>
         <v>3.1111111111111112</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>58</v>
       </c>
       <c r="B17" t="s">
@@ -2861,13 +2885,13 @@
         <v>83</v>
       </c>
       <c r="E17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
       <c r="G17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -2879,7 +2903,8 @@
         <v>2</v>
       </c>
       <c r="K17">
-        <v>9</v>
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="L17">
         <v>16</v>
@@ -2912,8 +2937,8 @@
         <v>4</v>
       </c>
       <c r="V17">
-        <f t="shared" si="0"/>
-        <v>25</v>
+        <f t="shared" si="1"/>
+        <v>27</v>
       </c>
       <c r="W17" s="1">
         <v>0.16</v>
@@ -2940,15 +2965,16 @@
         <v>6</v>
       </c>
       <c r="AE17">
-        <v>25</v>
+        <f t="shared" si="2"/>
+        <v>27</v>
       </c>
       <c r="AF17">
         <f>AVERAGE(2,5,5,2,2,2,2,2,2)</f>
         <v>2.6666666666666665</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>60</v>
       </c>
       <c r="B18" t="s">
@@ -2976,10 +3002,11 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
       <c r="L18">
         <v>18</v>
@@ -3012,8 +3039,8 @@
         <v>18</v>
       </c>
       <c r="V18">
-        <f t="shared" si="0"/>
-        <v>29</v>
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
       <c r="W18" s="1">
         <v>0</v>
@@ -3040,15 +3067,16 @@
         <v>5</v>
       </c>
       <c r="AE18">
-        <v>29</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="AF18">
         <f>AVERAGE(6,2,3,2,2,2,2,2,3,2,2)</f>
         <v>2.5454545454545454</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
         <v>63</v>
       </c>
       <c r="B19" t="s">
@@ -3061,28 +3089,29 @@
         <v>83</v>
       </c>
       <c r="E19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
       <c r="G19">
+        <v>4</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>1</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <v>10</v>
-      </c>
       <c r="L19">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M19" s="1">
         <v>0.3</v>
@@ -3112,8 +3141,8 @@
         <v>10</v>
       </c>
       <c r="V19">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>17</v>
       </c>
       <c r="W19" s="1">
         <v>0.15</v>
@@ -3137,18 +3166,19 @@
         <v>0.5</v>
       </c>
       <c r="AD19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AE19">
-        <v>20</v>
+        <f t="shared" si="2"/>
+        <v>17</v>
       </c>
       <c r="AF19">
         <f>AVERAGE(5,2,2,3,2,2)</f>
         <v>2.6666666666666665</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
         <v>66</v>
       </c>
       <c r="B20" t="s">
@@ -3164,25 +3194,26 @@
         <v>4</v>
       </c>
       <c r="F20">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G20">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="I20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J20">
         <v>0</v>
       </c>
       <c r="K20">
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
       <c r="L20">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="M20" s="1">
         <v>0.2</v>
@@ -3212,8 +3243,8 @@
         <v>8</v>
       </c>
       <c r="V20">
-        <f t="shared" si="0"/>
-        <v>49</v>
+        <f t="shared" si="1"/>
+        <v>41</v>
       </c>
       <c r="W20" s="1">
         <v>0.08</v>
@@ -3240,15 +3271,16 @@
         <v>9</v>
       </c>
       <c r="AE20">
-        <v>49</v>
+        <f t="shared" si="2"/>
+        <v>41</v>
       </c>
       <c r="AF20">
         <f>AVERAGE(3,2,3,3,4,1,6,2,2,2,1,6,2,2,2,2)</f>
         <v>2.6875</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
         <v>68</v>
       </c>
       <c r="B21" t="s">
@@ -3279,6 +3311,7 @@
         <v>0</v>
       </c>
       <c r="K21">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="L21">
@@ -3312,7 +3345,7 @@
         <v>10</v>
       </c>
       <c r="V21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="W21" s="1">
@@ -3340,6 +3373,7 @@
         <v>3</v>
       </c>
       <c r="AE21">
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="AF21">
@@ -3347,42 +3381,42 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="6"/>
-      <c r="S22" s="5"/>
-      <c r="T22" s="5"/>
-      <c r="U22" s="5"/>
-      <c r="V22" s="5"/>
-      <c r="W22" s="6"/>
-      <c r="X22" s="6"/>
-      <c r="Y22" s="6"/>
-      <c r="Z22" s="6"/>
-      <c r="AA22" s="6"/>
-      <c r="AB22" s="6"/>
-      <c r="AC22" s="6"/>
-      <c r="AD22" s="5"/>
-      <c r="AE22" s="5"/>
-      <c r="AF22" s="5"/>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
+      <c r="U22" s="4"/>
+      <c r="V22" s="4"/>
+      <c r="W22" s="5"/>
+      <c r="X22" s="5"/>
+      <c r="Y22" s="5"/>
+      <c r="Z22" s="5"/>
+      <c r="AA22" s="5"/>
+      <c r="AB22" s="5"/>
+      <c r="AC22" s="5"/>
+      <c r="AD22" s="4"/>
+      <c r="AE22" s="4"/>
+      <c r="AF22" s="4"/>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>71</v>
       </c>
       <c r="E23">
@@ -3391,84 +3425,84 @@
       </c>
       <c r="F23">
         <f>SUM(F2:F21)</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G23">
         <f>SUM(G2:G21)</f>
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H23">
         <f>SUM(H2:H21)</f>
         <v>2</v>
       </c>
       <c r="I23">
-        <f t="shared" ref="I23:L23" si="1">SUM(I2:I21)</f>
-        <v>21</v>
+        <f t="shared" ref="I23:L23" si="3">SUM(I2:I21)</f>
+        <v>19</v>
       </c>
       <c r="J23">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <f t="shared" si="3"/>
+        <v>9</v>
       </c>
       <c r="K23">
-        <f t="shared" si="1"/>
-        <v>153</v>
+        <f t="shared" si="3"/>
+        <v>148</v>
       </c>
       <c r="L23">
-        <f t="shared" si="1"/>
-        <v>262</v>
+        <f t="shared" si="3"/>
+        <v>259</v>
       </c>
       <c r="V23">
         <f>SUM(V2:V21)</f>
-        <v>415</v>
+        <v>407</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>72</v>
       </c>
       <c r="E24" s="1">
-        <f t="shared" ref="E24:J24" si="2">E23/153</f>
+        <f t="shared" ref="E24:J24" si="4">E23/153</f>
         <v>0.39215686274509803</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
+        <v>0.11764705882352941</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" si="4"/>
+        <v>0.26143790849673204</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="4"/>
+        <v>1.3071895424836602E-2</v>
+      </c>
+      <c r="I24" s="1">
+        <f t="shared" si="4"/>
         <v>0.12418300653594772</v>
       </c>
-      <c r="G24" s="1">
-        <f t="shared" si="2"/>
-        <v>0.28104575163398693</v>
-      </c>
-      <c r="H24" s="1">
-        <f t="shared" si="2"/>
-        <v>1.3071895424836602E-2</v>
-      </c>
-      <c r="I24" s="1">
-        <f t="shared" si="2"/>
-        <v>0.13725490196078433</v>
-      </c>
       <c r="J24" s="1">
-        <f t="shared" si="2"/>
-        <v>5.2287581699346407E-2</v>
+        <f t="shared" si="4"/>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="K24" s="1">
         <f>K23/415</f>
-        <v>0.36867469879518072</v>
+        <v>0.3566265060240964</v>
       </c>
       <c r="L24" s="1">
         <f>L23/415</f>
-        <v>0.63132530120481922</v>
+        <v>0.62409638554216873</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="K29" s="2"/>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="K31" s="2"/>
     </row>
   </sheetData>
@@ -3484,120 +3518,130 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1DB2BFF-5F3D-42B3-B778-040C1DE270B9}">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <f>SUM(python_codes_analysis!E6:F6)</f>
+        <v>11</v>
       </c>
       <c r="C2">
+        <f>SUM(python_codes_analysis!G6:H6)</f>
         <v>5</v>
       </c>
       <c r="D2">
+        <f>SUM(python_codes_analysis!J6)</f>
         <v>0</v>
       </c>
       <c r="E2">
+        <f>SUM(python_codes_analysis!I6)</f>
         <v>4</v>
       </c>
       <c r="F2">
-        <v>19</v>
+        <f>SUM(B2:E2)</f>
+        <v>20</v>
       </c>
       <c r="G2">
-        <v>30</v>
+        <f>SUM(python_codes_analysis!L6)</f>
+        <v>33</v>
       </c>
       <c r="H2">
         <f>SUM(F2:G2)</f>
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="I2" s="2">
         <f>(B2/F2)</f>
-        <v>0.52631578947368418</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J2" s="2">
         <f>(C2/F2)</f>
-        <v>0.26315789473684209</v>
+        <v>0.25</v>
       </c>
       <c r="K2" s="2">
         <f>(D2/F2)</f>
@@ -3605,63 +3649,70 @@
       </c>
       <c r="L2" s="2">
         <f>(E2/F2)</f>
-        <v>0.21052631578947367</v>
+        <v>0.2</v>
       </c>
       <c r="M2" s="2">
         <f>(F2/H2)</f>
-        <v>0.38775510204081631</v>
+        <v>0.37735849056603776</v>
       </c>
       <c r="N2" s="2">
         <f>(G2/H2)</f>
-        <v>0.61224489795918369</v>
+        <v>0.62264150943396224</v>
       </c>
       <c r="O2">
         <v>1</v>
       </c>
       <c r="P2">
+        <f>SUM(python_codes_analysis!AD6)/O2</f>
         <v>9</v>
       </c>
       <c r="Q2">
         <v>2.5263157894736841</v>
       </c>
-      <c r="R2" s="7">
+      <c r="R2" s="6">
         <f>(SUM(F2:G2))/O2</f>
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>64</v>
       </c>
       <c r="B3">
-        <v>14</v>
+        <f>SUM(python_codes_analysis!E19:F20)</f>
+        <v>12</v>
       </c>
       <c r="C3">
-        <v>11</v>
+        <f>SUM(python_codes_analysis!G19:H20)</f>
+        <v>6</v>
       </c>
       <c r="D3">
+        <f>SUM(python_codes_analysis!J19:J20)</f>
         <v>0</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <f>SUM(python_codes_analysis!I19:I20)</f>
+        <v>3</v>
       </c>
       <c r="F3">
-        <v>30</v>
+        <f>SUM(B3:E3)</f>
+        <v>21</v>
       </c>
       <c r="G3">
-        <v>39</v>
+        <f>SUM(python_codes_analysis!L19:L20)</f>
+        <v>37</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H10" si="0">SUM(F3:G3)</f>
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="I3" s="2">
         <f t="shared" ref="I3:I10" si="1">(B3/F3)</f>
-        <v>0.46666666666666667</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="J3" s="2">
         <f t="shared" ref="J3:J10" si="2">(C3/F3)</f>
-        <v>0.36666666666666664</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="K3" s="2">
         <f t="shared" ref="K3:K10" si="3">(D3/F3)</f>
@@ -3669,67 +3720,74 @@
       </c>
       <c r="L3" s="2">
         <f t="shared" ref="L3:L10" si="4">(E3/F3)</f>
-        <v>0.16666666666666666</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="M3" s="2">
         <f t="shared" ref="M3:M10" si="5">(F3/H3)</f>
-        <v>0.43478260869565216</v>
+        <v>0.36206896551724138</v>
       </c>
       <c r="N3" s="2">
         <f t="shared" ref="N3:N10" si="6">(G3/H3)</f>
-        <v>0.56521739130434778</v>
+        <v>0.63793103448275867</v>
       </c>
       <c r="O3">
         <v>2</v>
       </c>
-      <c r="P3">
-        <v>7</v>
+      <c r="P3" s="6">
+        <f>SUM(python_codes_analysis!AD19:AD20)/O3</f>
+        <v>6.5</v>
       </c>
       <c r="Q3">
         <v>2.677083333333333</v>
       </c>
-      <c r="R3" s="7">
+      <c r="R3" s="6">
         <f t="shared" ref="R3:R5" si="7">(SUM(F3:G3))/O3</f>
-        <v>34.5</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>61</v>
       </c>
       <c r="B4">
+        <f>SUM(python_codes_analysis!E18:F18)</f>
         <v>3</v>
       </c>
       <c r="C4">
+        <f>SUM(python_codes_analysis!G18:H18)</f>
         <v>8</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <f>SUM(python_codes_analysis!J18)</f>
+        <v>1</v>
       </c>
       <c r="E4">
+        <f>SUM(python_codes_analysis!I18)</f>
         <v>0</v>
       </c>
       <c r="F4">
-        <v>11</v>
+        <f t="shared" ref="F4:F10" si="8">SUM(B4:E4)</f>
+        <v>12</v>
       </c>
       <c r="G4">
+        <f>SUM(python_codes_analysis!L18)</f>
         <v>18</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I4" s="2">
         <f t="shared" si="1"/>
-        <v>0.27272727272727271</v>
+        <v>0.25</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" si="2"/>
-        <v>0.72727272727272729</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="K4" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="L4" s="2">
         <f t="shared" si="4"/>
@@ -3737,123 +3795,137 @@
       </c>
       <c r="M4" s="2">
         <f t="shared" si="5"/>
-        <v>0.37931034482758619</v>
+        <v>0.4</v>
       </c>
       <c r="N4" s="2">
         <f t="shared" si="6"/>
-        <v>0.62068965517241381</v>
+        <v>0.6</v>
       </c>
       <c r="O4">
         <v>1</v>
       </c>
       <c r="P4">
+        <f>SUM(python_codes_analysis!AD18)/O4</f>
         <v>5</v>
       </c>
-      <c r="Q4" s="8">
+      <c r="Q4" s="7">
         <v>2.5454545454545454</v>
       </c>
-      <c r="R4" s="7">
+      <c r="R4" s="6">
+        <f t="shared" si="7"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5">
+        <f>SUM(python_codes_analysis!E16:F17)</f>
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <f>SUM(python_codes_analysis!G16:H17)</f>
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <f>SUM(python_codes_analysis!J16:J17)</f>
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <f>SUM(python_codes_analysis!I16:I17)</f>
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="8"/>
+        <v>22</v>
+      </c>
+      <c r="G5">
+        <f>SUM(python_codes_analysis!L16:L17)</f>
+        <v>36</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="1"/>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" si="2"/>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="K5" s="2">
+        <f t="shared" si="3"/>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="L5" s="2">
+        <f t="shared" si="4"/>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="M5" s="2">
+        <f t="shared" si="5"/>
+        <v>0.37931034482758619</v>
+      </c>
+      <c r="N5" s="2">
+        <f t="shared" si="6"/>
+        <v>0.62068965517241381</v>
+      </c>
+      <c r="O5">
+        <v>2</v>
+      </c>
+      <c r="P5">
+        <f>SUM(python_codes_analysis!AD16:AD17)/O5</f>
+        <v>6</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>2.8888888888888888</v>
+      </c>
+      <c r="R5" s="6">
         <f t="shared" si="7"/>
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>18</v>
-      </c>
-      <c r="G5">
-        <v>36</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="I5" s="2">
-        <f t="shared" si="1"/>
-        <v>0.44444444444444442</v>
-      </c>
-      <c r="J5" s="2">
-        <f t="shared" si="2"/>
-        <v>0.22222222222222221</v>
-      </c>
-      <c r="K5" s="2">
-        <f t="shared" si="3"/>
-        <v>0.22222222222222221</v>
-      </c>
-      <c r="L5" s="2">
-        <f t="shared" si="4"/>
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="M5" s="2">
-        <f t="shared" si="5"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="N5" s="2">
-        <f t="shared" si="6"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="O5">
-        <v>2</v>
-      </c>
-      <c r="P5">
-        <v>6</v>
-      </c>
-      <c r="Q5" s="8">
-        <v>2.8888888888888888</v>
-      </c>
-      <c r="R5" s="7">
-        <f t="shared" si="7"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
       <c r="B6">
+        <f>SUM(python_codes_analysis!E2:F2)</f>
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <f>SUM(python_codes_analysis!G2:H2)</f>
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <f>SUM(python_codes_analysis!J2)</f>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f>SUM(python_codes_analysis!I2)</f>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>6</v>
-      </c>
       <c r="G6">
-        <v>12</v>
+        <f>SUM(python_codes_analysis!L2)</f>
+        <v>8</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I6" s="2">
         <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="K6" s="2">
         <f t="shared" si="3"/>
@@ -3874,37 +3946,44 @@
       <c r="O6">
         <v>1</v>
       </c>
-      <c r="P6" s="7">
+      <c r="P6" s="6">
+        <f>SUM(python_codes_analysis!AD2)/O6</f>
         <v>4</v>
       </c>
-      <c r="Q6" s="8">
+      <c r="Q6" s="7">
         <v>2.8333333333333335</v>
       </c>
-      <c r="R6" s="7">
+      <c r="R6" s="6">
         <f>(SUM(F6:G6))/O6</f>
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
       <c r="B7">
+        <f>SUM(python_codes_analysis!E7:F14)</f>
         <v>30</v>
       </c>
       <c r="C7">
+        <f>SUM(python_codes_analysis!G7:H14)</f>
         <v>9</v>
       </c>
       <c r="D7">
+        <f>SUM(python_codes_analysis!J7:J14)</f>
         <v>3</v>
       </c>
       <c r="E7">
+        <f>SUM(python_codes_analysis!I7:I14)</f>
         <v>10</v>
       </c>
       <c r="F7">
+        <f t="shared" si="8"/>
         <v>52</v>
       </c>
       <c r="G7">
+        <f>SUM(python_codes_analysis!L7:L14)</f>
         <v>85</v>
       </c>
       <c r="H7">
@@ -3938,37 +4017,44 @@
       <c r="O7">
         <v>8</v>
       </c>
-      <c r="P7" s="7">
+      <c r="P7" s="6">
+        <f>SUM(python_codes_analysis!AD7:AD14)/O7</f>
         <v>4.875</v>
       </c>
-      <c r="Q7" s="8">
+      <c r="Q7" s="7">
         <v>2.4330357142857144</v>
       </c>
-      <c r="R7" s="7">
+      <c r="R7" s="6">
         <f>(SUM(F7:G7))/O7</f>
         <v>17.125</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>69</v>
       </c>
       <c r="B8">
+        <f>SUM(python_codes_analysis!E21:F21)</f>
         <v>5</v>
       </c>
       <c r="C8">
+        <f>SUM(python_codes_analysis!G21:H21)</f>
         <v>1</v>
       </c>
       <c r="D8">
+        <f>SUM(python_codes_analysis!J21)</f>
         <v>0</v>
       </c>
       <c r="E8">
+        <f>SUM(python_codes_analysis!I21)</f>
         <v>0</v>
       </c>
       <c r="F8">
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="G8">
+        <f>SUM(python_codes_analysis!L21)</f>
         <v>10</v>
       </c>
       <c r="H8">
@@ -4003,36 +4089,43 @@
         <v>1</v>
       </c>
       <c r="P8">
+        <f>SUM(python_codes_analysis!AD21)/O8</f>
         <v>3</v>
       </c>
-      <c r="Q8" s="8">
+      <c r="Q8" s="7">
         <v>2.5</v>
       </c>
-      <c r="R8" s="7">
+      <c r="R8" s="6">
         <f>(SUM(F8:G8))/O8</f>
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
       <c r="B9">
+        <f>SUM(python_codes_analysis!E3:F5)</f>
         <v>3</v>
       </c>
       <c r="C9">
+        <f>SUM(python_codes_analysis!G3:H5)</f>
         <v>5</v>
       </c>
       <c r="D9">
+        <f>SUM(python_codes_analysis!J3:J5)</f>
         <v>0</v>
       </c>
       <c r="E9">
+        <f>SUM(python_codes_analysis!I3:I5)</f>
         <v>0</v>
       </c>
       <c r="F9">
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="G9">
+        <f>SUM(python_codes_analysis!L3:L5)</f>
         <v>27</v>
       </c>
       <c r="H9">
@@ -4067,36 +4160,43 @@
         <v>3</v>
       </c>
       <c r="P9">
+        <f>SUM(python_codes_analysis!AD3:AD5)/O9</f>
         <v>3</v>
       </c>
-      <c r="Q9" s="8">
+      <c r="Q9" s="7">
         <v>4.416666666666667</v>
       </c>
-      <c r="R9" s="7">
+      <c r="R9" s="6">
         <f>(SUM(F9:G9))/O9</f>
         <v>11.666666666666666</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>102</v>
       </c>
       <c r="B10">
+        <f>SUM(python_codes_analysis!E15:F15)</f>
         <v>2</v>
       </c>
       <c r="C10">
+        <f>SUM(python_codes_analysis!G15:H15)</f>
         <v>0</v>
       </c>
       <c r="D10">
+        <f>SUM(python_codes_analysis!J15)</f>
         <v>1</v>
       </c>
       <c r="E10">
+        <f>SUM(python_codes_analysis!I15)</f>
         <v>0</v>
       </c>
       <c r="F10">
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="G10">
+        <f>SUM(python_codes_analysis!L15)</f>
         <v>5</v>
       </c>
       <c r="H10">
@@ -4130,92 +4230,93 @@
       <c r="O10">
         <v>1</v>
       </c>
-      <c r="P10" s="7">
-        <v>3</v>
-      </c>
-      <c r="Q10" s="8">
+      <c r="P10" s="6">
+        <f>SUM(python_codes_analysis!AD15)/O10</f>
+        <v>4</v>
+      </c>
+      <c r="Q10" s="7">
         <v>2.3333333333333335</v>
       </c>
-      <c r="R10" s="7">
+      <c r="R10" s="6">
         <f>(SUM(F10:G10))/O10</f>
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>101</v>
       </c>
       <c r="B12">
-        <f>SUM(B2:B10)</f>
-        <v>79</v>
+        <f t="shared" ref="B12:H12" si="9">SUM(B2:B10)</f>
+        <v>78</v>
       </c>
       <c r="C12">
-        <f>SUM(C2:C10)</f>
-        <v>45</v>
+        <f t="shared" si="9"/>
+        <v>42</v>
       </c>
       <c r="D12">
-        <f>SUM(D2:D10)</f>
-        <v>8</v>
+        <f t="shared" si="9"/>
+        <v>9</v>
       </c>
       <c r="E12">
-        <f>SUM(E2:E10)</f>
-        <v>21</v>
+        <f t="shared" si="9"/>
+        <v>19</v>
       </c>
       <c r="F12">
-        <f>SUM(F2:F10)</f>
-        <v>153</v>
+        <f t="shared" si="9"/>
+        <v>148</v>
       </c>
       <c r="G12">
-        <f>SUM(G2:G10)</f>
-        <v>262</v>
+        <f t="shared" si="9"/>
+        <v>259</v>
       </c>
       <c r="H12">
-        <f>SUM(H2:H10)</f>
-        <v>415</v>
+        <f t="shared" si="9"/>
+        <v>407</v>
       </c>
       <c r="I12" s="2">
         <f>B12/F12</f>
-        <v>0.5163398692810458</v>
+        <v>0.52702702702702697</v>
       </c>
       <c r="J12" s="2">
         <f>C12/F12</f>
-        <v>0.29411764705882354</v>
+        <v>0.28378378378378377</v>
       </c>
       <c r="K12" s="2">
         <f>D12/F12</f>
-        <v>5.2287581699346407E-2</v>
+        <v>6.0810810810810814E-2</v>
       </c>
       <c r="L12" s="2">
         <f>E12/F12</f>
-        <v>0.13725490196078433</v>
+        <v>0.12837837837837837</v>
       </c>
       <c r="M12" s="2">
         <f>F12/H12</f>
-        <v>0.36867469879518072</v>
+        <v>0.36363636363636365</v>
       </c>
       <c r="N12" s="2">
         <f>G12/H12</f>
-        <v>0.63132530120481922</v>
+        <v>0.63636363636363635</v>
       </c>
     </row>
   </sheetData>

</xml_diff>